<commit_message>
AQT BETA V1.0 - Major interface update
</commit_message>
<xml_diff>
--- a/data/databaseAQT.xlsx
+++ b/data/databaseAQT.xlsx
@@ -600,7 +600,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +612,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -653,8 +659,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -987,7 +993,7 @@
     <col min="9" max="9" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1020,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1041,7 +1047,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1068,7 +1074,7 @@
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1095,7 +1101,7 @@
       </c>
       <c r="I4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1122,7 +1128,7 @@
       </c>
       <c r="I5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1149,7 +1155,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1176,7 +1182,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1203,7 +1209,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1230,7 +1236,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1257,7 +1263,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1284,7 +1290,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1311,7 +1317,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1338,7 +1344,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1365,7 +1371,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1392,7 +1398,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1419,7 +1425,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1446,7 +1452,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1473,7 +1479,7 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1500,7 +1506,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1527,7 +1533,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1554,7 +1560,7 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1581,7 +1587,7 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1608,7 +1614,7 @@
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1635,7 +1641,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1662,7 +1668,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1689,7 +1695,7 @@
       </c>
       <c r="I26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1">
         <v>26</v>
       </c>

</xml_diff>